<commit_message>
feat: add trialDistributions_exp2.xls data
</commit_message>
<xml_diff>
--- a/extra_data_trial_distributions/trialDistributions_exp2.xlsx
+++ b/extra_data_trial_distributions/trialDistributions_exp2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanknights/Library/Mobile Documents/com~apple~CloudDocs/owncloud/projects/UEA/neglect/article_2023/src_data/TrialDistributions-Experiment2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanknights/PycharmProjects/neglect/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E879E444-CAAC-2245-AC8F-050805686ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC58E555-981A-F448-A393-6073B1D8A567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20060" windowHeight="11620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20060" windowHeight="11620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="6" r:id="rId1"/>
@@ -494,8 +494,8 @@
   </sheetPr>
   <dimension ref="A1:AC12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1010,6 +1010,18 @@
       <c r="I12">
         <v>9</v>
       </c>
+      <c r="J12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
+      <c r="M12">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1024,7 +1036,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1523,6 +1535,18 @@
       <c r="I12">
         <v>1</v>
       </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1537,7 +1561,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2036,6 +2060,18 @@
       <c r="I12">
         <v>0</v>
       </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2049,8 +2085,8 @@
   </sheetPr>
   <dimension ref="A1:AC12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2568,6 +2604,18 @@
       <c r="I12">
         <v>0</v>
       </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2582,7 +2630,7 @@
   <dimension ref="A1:AC12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3100,6 +3148,18 @@
       <c r="I12">
         <v>9</v>
       </c>
+      <c r="J12">
+        <v>9</v>
+      </c>
+      <c r="K12">
+        <v>9</v>
+      </c>
+      <c r="L12">
+        <v>9</v>
+      </c>
+      <c r="M12">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add trial distribtution functions (fixed all matching vals error)
</commit_message>
<xml_diff>
--- a/extra_data_trial_distributions/trialDistributions_exp2.xlsx
+++ b/extra_data_trial_distributions/trialDistributions_exp2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanknights/PycharmProjects/neglect/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanknights/PycharmProjects/neglect/extra_data_trial_distributions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC58E555-981A-F448-A393-6073B1D8A567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F79A56-4F79-AC47-BCFF-6D2204906DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20060" windowHeight="11620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20060" windowHeight="11620" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="6" r:id="rId1"/>
@@ -492,10 +492,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:AC12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:CG1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -515,7 +515,7 @@
     <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,24 +555,8 @@
       <c r="M1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -613,7 +597,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -654,7 +638,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -695,7 +679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -736,7 +720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -777,7 +761,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -818,7 +802,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -859,7 +843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -900,7 +884,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -941,7 +925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -982,7 +966,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1035,8 +1019,8 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:AT1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1560,8 +1544,8 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:AZ1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2083,10 +2067,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:AC12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:BK1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2104,12 +2088,9 @@
     <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5" customWidth="1"/>
-    <col min="23" max="23" width="14.1640625" customWidth="1"/>
-    <col min="28" max="28" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2149,24 +2130,8 @@
       <c r="M1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2207,7 +2172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2248,7 +2213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2289,7 +2254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2330,7 +2295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2371,7 +2336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2412,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2453,7 +2418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2494,7 +2459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2535,7 +2500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -2576,7 +2541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -2627,10 +2592,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:AC12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:BD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2648,12 +2613,9 @@
     <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5" customWidth="1"/>
-    <col min="23" max="23" width="14.1640625" customWidth="1"/>
-    <col min="28" max="28" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2693,24 +2655,8 @@
       <c r="M1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2751,7 +2697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2792,7 +2738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2833,7 +2779,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2874,7 +2820,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2915,7 +2861,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2956,7 +2902,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2997,7 +2943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3038,7 +2984,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -3079,7 +3025,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -3120,7 +3066,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>

</xml_diff>